<commit_message>
Started Work on Fractal Dimension
</commit_message>
<xml_diff>
--- a/Tutorials/Formulas.xlsx
+++ b/Tutorials/Formulas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aadit\Documents\GitHub\mCNV-image-analysis\Tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93126E98-BEA5-48E6-9982-74C29955DCBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812CD5F0-C91D-48AF-9AE3-FB5C7E4C573D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -261,8 +261,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -284,6 +282,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -569,7 +569,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,10 +580,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
@@ -620,24 +620,24 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="20" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="18"/>
+      <c r="B8" s="16"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="17" t="s">
         <v>12</v>
       </c>
     </row>
@@ -645,7 +645,7 @@
       <c r="A10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -653,15 +653,15 @@
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="18" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="15" t="s">
         <v>16</v>
       </c>
     </row>
@@ -669,13 +669,13 @@
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="14"/>
+      <c r="B14" s="12"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="15" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>